<commit_message>
progress report 7 updated model
</commit_message>
<xml_diff>
--- a/forecast_eval/mae_VAR_by_seasonality_financial&demand.xlsx
+++ b/forecast_eval/mae_VAR_by_seasonality_financial&demand.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nicole Dropbox\Dropbox\_GEORGETOWN Dropbox\_Hoya1\Hoya1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nicole Dropbox\Dropbox\_GEORGETOWN Dropbox\_Hoya1\Hoya1\forecast_eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D6AFF-A30C-4D20-A6AC-1E6EF8932E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C268968D-21B6-40ED-BE4B-74587D02BD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="970" windowWidth="34120" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3370" yWindow="1530" windowWidth="34120" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mae_VAR_by_seasonality_financia" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -120,6 +119,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,9 +582,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1152,7 +1155,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K16"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1797,7 +1800,7 @@
         <f t="shared" si="1"/>
         <v>15.000823068809876</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <f t="shared" si="1"/>
         <v>12.3227440314796</v>
       </c>
@@ -1842,7 +1845,7 @@
         <f t="shared" si="2"/>
         <v>1.0000548712539916</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
         <v>0.82151626876530659</v>
       </c>

</xml_diff>